<commit_message>
Update yn_to_tf spec reader helper function to be more robust
</commit_message>
<xml_diff>
--- a/tests/testthat/example_spec.xlsx
+++ b/tests/testthat/example_spec.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://atorusresearchcom.sharepoint.com/sites/GSKAtorusOpenSourceCollaboration/Shared Documents/Metadata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\16105\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="16" documentId="8_{B9AAB146-600D-4A4F-8267-EA23D77E5D9C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{2DEE3E64-B370-4D31-B5F2-69BA952F3342}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73C88E04-8351-45C0-A7BC-8DDFCC3970DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{55B6BB6F-AC0C-4433-8374-B7E8883D4B64}"/>
+    <workbookView xWindow="34005" yWindow="1605" windowWidth="21600" windowHeight="11160" xr2:uid="{55B6BB6F-AC0C-4433-8374-B7E8883D4B64}"/>
   </bookViews>
   <sheets>
     <sheet name="DM" sheetId="4" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="91">
   <si>
     <t>DOMAIN</t>
   </si>
@@ -298,6 +298,21 @@
   </si>
   <si>
     <t>SUPP</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>YES</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>NO</t>
   </si>
 </sst>
 </file>
@@ -669,8 +684,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C32AC68-62D7-4A7F-8B27-87CD8F0E9B4D}">
   <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1164,7 +1179,7 @@
   <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1220,7 +1235,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>29</v>
+        <v>86</v>
       </c>
       <c r="D2" t="s">
         <v>13</v>
@@ -1249,7 +1264,7 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>29</v>
+        <v>87</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -1307,7 +1322,7 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>29</v>
+        <v>89</v>
       </c>
       <c r="D5" t="s">
         <v>15</v>
@@ -1464,7 +1479,7 @@
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="D10" t="s">
         <v>21</v>
@@ -1748,8 +1763,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4C3DEF1-0091-4B98-BC83-2E06A6B17943}">
   <dimension ref="A1:L16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2053,7 +2068,7 @@
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="E10" t="s">
         <v>21</v>
@@ -2249,21 +2264,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100EB6E4C2F97031D489E3E77B0BE03700D" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="004272f6834ec76c6281332d2d4c0598">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="5cc28008-2883-42ef-8e17-9df6c4ad1700" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0560789715acdc8994f3be0578f8599b" ns2:_="">
     <xsd:import namespace="5cc28008-2883-42ef-8e17-9df6c4ad1700"/>
@@ -2435,31 +2435,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B843AB3F-AC2C-4D7C-A0BB-5A16DBE70CF4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="5cc28008-2883-42ef-8e17-9df6c4ad1700"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C601B812-8BE1-4990-9F7D-FC49A7E87FE7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D7A85C7C-B6DE-44A7-9E67-256BDA77440A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2475,4 +2466,28 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C601B812-8BE1-4990-9F7D-FC49A7E87FE7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B843AB3F-AC2C-4D7C-A0BB-5A16DBE70CF4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="5cc28008-2883-42ef-8e17-9df6c4ad1700"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>